<commit_message>
adicionado cantidad de engranajes
</commit_message>
<xml_diff>
--- a/Lista.xlsx
+++ b/Lista.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Tesis MM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ibngary\TrenEngranajes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DCBFB59-8E19-4FC7-8BC9-F9F995CCE675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC20966-AA31-4C75-AE5C-C73F39C50B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6377255A-99EC-487A-B6CD-D3B984F02E04}"/>
   </bookViews>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2C1074-C4AF-4E21-A50D-72970AC44A1F}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,26 +431,330 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>32</v>
       </c>
-      <c r="B4">
+      <c r="B7">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>55</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>61</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>62</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>64</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>66</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>70</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>71</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>72</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>73</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>74</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>76</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>79</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>80</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>84</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>86</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>88</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>90</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>96</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>100</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>